<commit_message>
*from server. update vedomost
</commit_message>
<xml_diff>
--- a/months/nov23/nov23.xlsx
+++ b/months/nov23/nov23.xlsx
@@ -4135,7 +4135,11 @@
       <c r="B15" t="n">
         <v>2</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>ELza</t>
@@ -4330,7 +4334,11 @@
       <c r="B16" t="n">
         <v>3</v>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>Lza, E</t>
@@ -4373,14 +4381,46 @@
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
-      <c r="AG16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>can`t</t>
+        </is>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>23:09</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="AH16" t="inlineStr"/>
       <c r="AI16" t="inlineStr"/>
       <c r="AJ16" t="inlineStr"/>

</xml_diff>